<commit_message>
Fixed Hole in Reactor Top
</commit_message>
<xml_diff>
--- a/Photobioreactor/Reactor_rev1/Parts_Needed.xlsx
+++ b/Photobioreactor/Reactor_rev1/Parts_Needed.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A585C468-AE1A-4F95-830E-294A85CE07BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CA268B-BCE7-4098-9B77-7FFF3AF5CE47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22256" windowHeight="12641" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Magnets</t>
   </si>
@@ -53,6 +53,21 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Arctic</t>
+  </si>
+  <si>
+    <t>Jar</t>
+  </si>
+  <si>
+    <t>1590ml</t>
+  </si>
+  <si>
+    <t>Weck</t>
   </si>
 </sst>
 </file>
@@ -373,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -384,9 +399,10 @@
     <col min="1" max="1" width="15.58203125" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
     <col min="3" max="3" width="14.58203125" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -396,8 +412,11 @@
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -418,8 +437,11 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -430,7 +452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -439,6 +461,20 @@
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>